<commit_message>
obj 1 report complete
</commit_message>
<xml_diff>
--- a/Schedule Objective 2/patientdata_objective_2.xlsx
+++ b/Schedule Objective 2/patientdata_objective_2.xlsx
@@ -13,7 +13,1132 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1504" uniqueCount="1500">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1880" uniqueCount="1875">
+  <si>
+    <t>Room_No</t>
+  </si>
+  <si>
+    <t>Available_Interval</t>
+  </si>
+  <si>
+    <t>(0,60)</t>
+  </si>
+  <si>
+    <t>(20,180)</t>
+  </si>
+  <si>
+    <t>(60,220)</t>
+  </si>
+  <si>
+    <t>(180,360)</t>
+  </si>
+  <si>
+    <t>(280,460)</t>
+  </si>
+  <si>
+    <t>(400,480)</t>
+  </si>
+  <si>
+    <t>(0,140)</t>
+  </si>
+  <si>
+    <t>(40,160)</t>
+  </si>
+  <si>
+    <t>(120,260)</t>
+  </si>
+  <si>
+    <t>(240,340)</t>
+  </si>
+  <si>
+    <t>(240,400)</t>
+  </si>
+  <si>
+    <t>(320,480)</t>
+  </si>
+  <si>
+    <t>(20,40)</t>
+  </si>
+  <si>
+    <t>(80,180)</t>
+  </si>
+  <si>
+    <t>(140,220)</t>
+  </si>
+  <si>
+    <t>(160,260)</t>
+  </si>
+  <si>
+    <t>(260,340)</t>
+  </si>
+  <si>
+    <t>(280,360)</t>
+  </si>
+  <si>
+    <t>(340,480)</t>
+  </si>
+  <si>
+    <t>(0,20)</t>
+  </si>
+  <si>
+    <t>(0,200)</t>
+  </si>
+  <si>
+    <t>(100,380)</t>
+  </si>
+  <si>
+    <t>(240,340)</t>
+  </si>
+  <si>
+    <t>(280,440)</t>
+  </si>
+  <si>
+    <t>(320,480)</t>
+  </si>
+  <si>
+    <t>(0,160)</t>
+  </si>
+  <si>
+    <t>(60,220)</t>
+  </si>
+  <si>
+    <t>(160,280)</t>
+  </si>
+  <si>
+    <t>(280,360)</t>
+  </si>
+  <si>
+    <t>(240,440)</t>
+  </si>
+  <si>
+    <t>(0,40)</t>
+  </si>
+  <si>
+    <t>(20,180)</t>
+  </si>
+  <si>
+    <t>(120,220)</t>
+  </si>
+  <si>
+    <t>(80,180)</t>
+  </si>
+  <si>
+    <t>(180,260)</t>
+  </si>
+  <si>
+    <t>(320,460)</t>
+  </si>
+  <si>
+    <t>(0,120)</t>
+  </si>
+  <si>
+    <t>(40,220)</t>
+  </si>
+  <si>
+    <t>(160,260)</t>
+  </si>
+  <si>
+    <t>(240,400)</t>
+  </si>
+  <si>
+    <t>(320,360)</t>
+  </si>
+  <si>
+    <t>(240,480)</t>
+  </si>
+  <si>
+    <t>(0,40)</t>
+  </si>
+  <si>
+    <t>(40,100)</t>
+  </si>
+  <si>
+    <t>(0,160)</t>
+  </si>
+  <si>
+    <t>(80,180)</t>
+  </si>
+  <si>
+    <t>(240,440)</t>
+  </si>
+  <si>
+    <t>(280,420)</t>
+  </si>
+  <si>
+    <t>(0,60)</t>
+  </si>
+  <si>
+    <t>(0,80)</t>
+  </si>
+  <si>
+    <t>(40,140)</t>
+  </si>
+  <si>
+    <t>(60,120)</t>
+  </si>
+  <si>
+    <t>(120,260)</t>
+  </si>
+  <si>
+    <t>(260,340)</t>
+  </si>
+  <si>
+    <t>(300,480)</t>
+  </si>
+  <si>
+    <t>(0,60)</t>
+  </si>
+  <si>
+    <t>(0,100)</t>
+  </si>
+  <si>
+    <t>(100,180)</t>
+  </si>
+  <si>
+    <t>(140,300)</t>
+  </si>
+  <si>
+    <t>(140,360)</t>
+  </si>
+  <si>
+    <t>(320,400)</t>
+  </si>
+  <si>
+    <t>(360,460)</t>
+  </si>
+  <si>
+    <t>(400,480)</t>
+  </si>
+  <si>
+    <t>(0,20)</t>
+  </si>
+  <si>
+    <t>(20,80)</t>
+  </si>
+  <si>
+    <t>(0,120)</t>
+  </si>
+  <si>
+    <t>(60,140)</t>
+  </si>
+  <si>
+    <t>(100,320)</t>
+  </si>
+  <si>
+    <t>(280,340)</t>
+  </si>
+  <si>
+    <t>(280,440)</t>
+  </si>
+  <si>
+    <t>(0,100)</t>
+  </si>
+  <si>
+    <t>(80,220)</t>
+  </si>
+  <si>
+    <t>(160,220)</t>
+  </si>
+  <si>
+    <t>(160,280)</t>
+  </si>
+  <si>
+    <t>(0,20)</t>
+  </si>
+  <si>
+    <t>(0,160)</t>
+  </si>
+  <si>
+    <t>(80,260)</t>
+  </si>
+  <si>
+    <t>(240,400)</t>
+  </si>
+  <si>
+    <t>(260,340)</t>
+  </si>
+  <si>
+    <t>(280,460)</t>
+  </si>
+  <si>
+    <t>(340,480)</t>
+  </si>
+  <si>
+    <t>(0,100)</t>
+  </si>
+  <si>
+    <t>(20,180)</t>
+  </si>
+  <si>
+    <t>(120,260)</t>
+  </si>
+  <si>
+    <t>(160,440)</t>
+  </si>
+  <si>
+    <t>(400,480)</t>
+  </si>
+  <si>
+    <t>(0,160)</t>
+  </si>
+  <si>
+    <t>(40,160)</t>
+  </si>
+  <si>
+    <t>(160,260)</t>
+  </si>
+  <si>
+    <t>(180,340)</t>
+  </si>
+  <si>
+    <t>(320,480)</t>
+  </si>
+  <si>
+    <t>Duration</t>
+  </si>
+  <si>
+    <t>Sched_Interval</t>
+  </si>
+  <si>
+    <t>(0,40)</t>
+  </si>
+  <si>
+    <t>(40,120)</t>
+  </si>
+  <si>
+    <t>(120,220)</t>
+  </si>
+  <si>
+    <t>(220,340)</t>
+  </si>
+  <si>
+    <t>(340,420)</t>
+  </si>
+  <si>
+    <t>(420,460)</t>
+  </si>
+  <si>
+    <t>(0,80)</t>
+  </si>
+  <si>
+    <t>(80,140)</t>
+  </si>
+  <si>
+    <t>(140,240)</t>
+  </si>
+  <si>
+    <t>(240,300)</t>
+  </si>
+  <si>
+    <t>(300,380)</t>
+  </si>
+  <si>
+    <t>(380,460)</t>
+  </si>
+  <si>
+    <t>(20,40)</t>
+  </si>
+  <si>
+    <t>(80,140)</t>
+  </si>
+  <si>
+    <t>(140,180)</t>
+  </si>
+  <si>
+    <t>(180,240)</t>
+  </si>
+  <si>
+    <t>(260,300)</t>
+  </si>
+  <si>
+    <t>(300,340)</t>
+  </si>
+  <si>
+    <t>(340,420)</t>
+  </si>
+  <si>
+    <t>(0,20)</t>
+  </si>
+  <si>
+    <t>(20,140)</t>
+  </si>
+  <si>
+    <t>(140,260)</t>
+  </si>
+  <si>
+    <t>(260,300)</t>
+  </si>
+  <si>
+    <t>(300,360)</t>
+  </si>
+  <si>
+    <t>(360,460)</t>
+  </si>
+  <si>
+    <t>(0,120)</t>
+  </si>
+  <si>
+    <t>(120,220)</t>
+  </si>
+  <si>
+    <t>(220,280)</t>
+  </si>
+  <si>
+    <t>(280,300)</t>
+  </si>
+  <si>
+    <t>(300,420)</t>
+  </si>
+  <si>
+    <t>(0,20)</t>
+  </si>
+  <si>
+    <t>(20,120)</t>
+  </si>
+  <si>
+    <t>(120,160)</t>
+  </si>
+  <si>
+    <t>(160,180)</t>
+  </si>
+  <si>
+    <t>(180,220)</t>
+  </si>
+  <si>
+    <t>(320,400)</t>
+  </si>
+  <si>
+    <t>(0,120)</t>
+  </si>
+  <si>
+    <t>(120,220)</t>
+  </si>
+  <si>
+    <t>(220,240)</t>
+  </si>
+  <si>
+    <t>(240,340)</t>
+  </si>
+  <si>
+    <t>(340,360)</t>
+  </si>
+  <si>
+    <t>(360,480)</t>
+  </si>
+  <si>
+    <t>(0,40)</t>
+  </si>
+  <si>
+    <t>(40,60)</t>
+  </si>
+  <si>
+    <t>(60,160)</t>
+  </si>
+  <si>
+    <t>(160,180)</t>
+  </si>
+  <si>
+    <t>(240,340)</t>
+  </si>
+  <si>
+    <t>(340,400)</t>
+  </si>
+  <si>
+    <t>(0,60)</t>
+  </si>
+  <si>
+    <t>(60,80)</t>
+  </si>
+  <si>
+    <t>(80,100)</t>
+  </si>
+  <si>
+    <t>(100,120)</t>
+  </si>
+  <si>
+    <t>(120,220)</t>
+  </si>
+  <si>
+    <t>(260,280)</t>
+  </si>
+  <si>
+    <t>(300,420)</t>
+  </si>
+  <si>
+    <t>(0,60)</t>
+  </si>
+  <si>
+    <t>(60,80)</t>
+  </si>
+  <si>
+    <t>(80,100)</t>
+  </si>
+  <si>
+    <t>(100,140)</t>
+  </si>
+  <si>
+    <t>(140,260)</t>
+  </si>
+  <si>
+    <t>(260,360)</t>
+  </si>
+  <si>
+    <t>(360,380)</t>
+  </si>
+  <si>
+    <t>(380,440)</t>
+  </si>
+  <si>
+    <t>(440,460)</t>
+  </si>
+  <si>
+    <t>(0,20)</t>
+  </si>
+  <si>
+    <t>(20,40)</t>
+  </si>
+  <si>
+    <t>(40,100)</t>
+  </si>
+  <si>
+    <t>(100,140)</t>
+  </si>
+  <si>
+    <t>(140,260)</t>
+  </si>
+  <si>
+    <t>(280,300)</t>
+  </si>
+  <si>
+    <t>(300,400)</t>
+  </si>
+  <si>
+    <t>(0,100)</t>
+  </si>
+  <si>
+    <t>(100,200)</t>
+  </si>
+  <si>
+    <t>(200,220)</t>
+  </si>
+  <si>
+    <t>(220,260)</t>
+  </si>
+  <si>
+    <t>(0,20)</t>
+  </si>
+  <si>
+    <t>(20,140)</t>
+  </si>
+  <si>
+    <t>(140,240)</t>
+  </si>
+  <si>
+    <t>(240,300)</t>
+  </si>
+  <si>
+    <t>(300,340)</t>
+  </si>
+  <si>
+    <t>(340,420)</t>
+  </si>
+  <si>
+    <t>(420,480)</t>
+  </si>
+  <si>
+    <t>(0,100)</t>
+  </si>
+  <si>
+    <t>(100,160)</t>
+  </si>
+  <si>
+    <t>(160,260)</t>
+  </si>
+  <si>
+    <t>(260,380)</t>
+  </si>
+  <si>
+    <t>(400,460)</t>
+  </si>
+  <si>
+    <t>(0,100)</t>
+  </si>
+  <si>
+    <t>(100,160)</t>
+  </si>
+  <si>
+    <t>(160,220)</t>
+  </si>
+  <si>
+    <t>(220,340)</t>
+  </si>
+  <si>
+    <t>(340,460)</t>
+  </si>
+  <si>
+    <t>Patient_Name</t>
+  </si>
+  <si>
+    <t>Anne</t>
+  </si>
+  <si>
+    <t>Cosmo</t>
+  </si>
+  <si>
+    <t>Milo</t>
+  </si>
+  <si>
+    <t>Daniel</t>
+  </si>
+  <si>
+    <t>Cillian</t>
+  </si>
+  <si>
+    <t>Bradley</t>
+  </si>
+  <si>
+    <t>Ezgi</t>
+  </si>
+  <si>
+    <t>Aras Bulut</t>
+  </si>
+  <si>
+    <t>Kenan</t>
+  </si>
+  <si>
+    <t>Serenay</t>
+  </si>
+  <si>
+    <t>Sherlock</t>
+  </si>
+  <si>
+    <t>Matt</t>
+  </si>
+  <si>
+    <t>Rosamund</t>
+  </si>
+  <si>
+    <t>Ata</t>
+  </si>
+  <si>
+    <t>Hannibal</t>
+  </si>
+  <si>
+    <t>Rachel</t>
+  </si>
+  <si>
+    <t>Walter</t>
+  </si>
+  <si>
+    <t>Haluk</t>
+  </si>
+  <si>
+    <t>Yıldız</t>
+  </si>
+  <si>
+    <t>Brad</t>
+  </si>
+  <si>
+    <t>Emma</t>
+  </si>
+  <si>
+    <t>Hugo</t>
+  </si>
+  <si>
+    <t>Gülse</t>
+  </si>
+  <si>
+    <t>Ali Rıza</t>
+  </si>
+  <si>
+    <t>Jake</t>
+  </si>
+  <si>
+    <t>Tom</t>
+  </si>
+  <si>
+    <t>Kıvanç</t>
+  </si>
+  <si>
+    <t>Ramsay</t>
+  </si>
+  <si>
+    <t>Özge</t>
+  </si>
+  <si>
+    <t>Margot</t>
+  </si>
+  <si>
+    <t>Joey</t>
+  </si>
+  <si>
+    <t>Hugh</t>
+  </si>
+  <si>
+    <t>Sezen</t>
+  </si>
+  <si>
+    <t>Chandler</t>
+  </si>
+  <si>
+    <t>Henry</t>
+  </si>
+  <si>
+    <t>Robert</t>
+  </si>
+  <si>
+    <t>Sylvester</t>
+  </si>
+  <si>
+    <t>Leonardo</t>
+  </si>
+  <si>
+    <t>James</t>
+  </si>
+  <si>
+    <t>Gregory</t>
+  </si>
+  <si>
+    <t>Cameron</t>
+  </si>
+  <si>
+    <t>Tyrion</t>
+  </si>
+  <si>
+    <t>Aleyna</t>
+  </si>
+  <si>
+    <t>Chris</t>
+  </si>
+  <si>
+    <t>Nihal</t>
+  </si>
+  <si>
+    <t>Angelina</t>
+  </si>
+  <si>
+    <t>Tom</t>
+  </si>
+  <si>
+    <t>Ralph</t>
+  </si>
+  <si>
+    <t>Jessica</t>
+  </si>
+  <si>
+    <t>İrem</t>
+  </si>
+  <si>
+    <t>Elçin</t>
+  </si>
+  <si>
+    <t>Hayko</t>
+  </si>
+  <si>
+    <t>Tarkan</t>
+  </si>
+  <si>
+    <t>Dwayne</t>
+  </si>
+  <si>
+    <t>Omar</t>
+  </si>
+  <si>
+    <t>Chris</t>
+  </si>
+  <si>
+    <t>Kate</t>
+  </si>
+  <si>
+    <t>Adam</t>
+  </si>
+  <si>
+    <t>Hande</t>
+  </si>
+  <si>
+    <t>Michael</t>
+  </si>
+  <si>
+    <t>Tom Marvolo</t>
+  </si>
+  <si>
+    <t>Bellatrix</t>
+  </si>
+  <si>
+    <t>Dave</t>
+  </si>
+  <si>
+    <t>Edward</t>
+  </si>
+  <si>
+    <t>Sansa</t>
+  </si>
+  <si>
+    <t>Hülya</t>
+  </si>
+  <si>
+    <t>Dwight</t>
+  </si>
+  <si>
+    <t>George</t>
+  </si>
+  <si>
+    <t>Jim</t>
+  </si>
+  <si>
+    <t>Frodo</t>
+  </si>
+  <si>
+    <t>Demet</t>
+  </si>
+  <si>
+    <t>Merve</t>
+  </si>
+  <si>
+    <t>Çağatay</t>
+  </si>
+  <si>
+    <t>Keira</t>
+  </si>
+  <si>
+    <t>Ivana</t>
+  </si>
+  <si>
+    <t>Milli Bobby</t>
+  </si>
+  <si>
+    <t>Cem</t>
+  </si>
+  <si>
+    <t>Natalie</t>
+  </si>
+  <si>
+    <t>Jackie</t>
+  </si>
+  <si>
+    <t>Fahriye</t>
+  </si>
+  <si>
+    <t>Justin</t>
+  </si>
+  <si>
+    <t>Jon</t>
+  </si>
+  <si>
+    <t>Bihter</t>
+  </si>
+  <si>
+    <t>Jerry</t>
+  </si>
+  <si>
+    <t>Murat</t>
+  </si>
+  <si>
+    <t>Marlon</t>
+  </si>
+  <si>
+    <t>Ana</t>
+  </si>
+  <si>
+    <t>Albus</t>
+  </si>
+  <si>
+    <t>Erşan</t>
+  </si>
+  <si>
+    <t>Tom</t>
+  </si>
+  <si>
+    <t>Murat</t>
+  </si>
+  <si>
+    <t>Burak</t>
+  </si>
+  <si>
+    <t>Patient_Surname</t>
+  </si>
+  <si>
+    <t>Hathaway</t>
+  </si>
+  <si>
+    <t>Kramer</t>
+  </si>
+  <si>
+    <t>Ventimiglia</t>
+  </si>
+  <si>
+    <t>Radcliffe</t>
+  </si>
+  <si>
+    <t>Murphy</t>
+  </si>
+  <si>
+    <t>Cooper</t>
+  </si>
+  <si>
+    <t>Mola</t>
+  </si>
+  <si>
+    <t>İynemli</t>
+  </si>
+  <si>
+    <t>Doğulu</t>
+  </si>
+  <si>
+    <t>Sarıkaya</t>
+  </si>
+  <si>
+    <t>Holmes</t>
+  </si>
+  <si>
+    <t>Damon</t>
+  </si>
+  <si>
+    <t>Pike</t>
+  </si>
+  <si>
+    <t>Demirer</t>
+  </si>
+  <si>
+    <t>Lecter</t>
+  </si>
+  <si>
+    <t>Green</t>
+  </si>
+  <si>
+    <t>White</t>
+  </si>
+  <si>
+    <t>Levent</t>
+  </si>
+  <si>
+    <t>Tilbe</t>
+  </si>
+  <si>
+    <t>Pitt</t>
+  </si>
+  <si>
+    <t>Watson</t>
+  </si>
+  <si>
+    <t>Weaving</t>
+  </si>
+  <si>
+    <t>Birsel</t>
+  </si>
+  <si>
+    <t>Tekin</t>
+  </si>
+  <si>
+    <t>Gyllenhaal</t>
+  </si>
+  <si>
+    <t>Hardy</t>
+  </si>
+  <si>
+    <t>Tatlıtuğ</t>
+  </si>
+  <si>
+    <t>Bolton</t>
+  </si>
+  <si>
+    <t>Özpirinççi</t>
+  </si>
+  <si>
+    <t>Robbie</t>
+  </si>
+  <si>
+    <t>Tribbiani</t>
+  </si>
+  <si>
+    <t>Jackman</t>
+  </si>
+  <si>
+    <t>Aksu</t>
+  </si>
+  <si>
+    <t>Bing</t>
+  </si>
+  <si>
+    <t>Cavill</t>
+  </si>
+  <si>
+    <t>Downey Jr.</t>
+  </si>
+  <si>
+    <t>Stallone</t>
+  </si>
+  <si>
+    <t>DiCaprio</t>
+  </si>
+  <si>
+    <t>Moriarty</t>
+  </si>
+  <si>
+    <t>House</t>
+  </si>
+  <si>
+    <t>Diaz</t>
+  </si>
+  <si>
+    <t>Lannister</t>
+  </si>
+  <si>
+    <t>Tilki</t>
+  </si>
+  <si>
+    <t>O'Dowd</t>
+  </si>
+  <si>
+    <t>Ziyagil</t>
+  </si>
+  <si>
+    <t>Jolie</t>
+  </si>
+  <si>
+    <t>Cruise</t>
+  </si>
+  <si>
+    <t>Fiennes</t>
+  </si>
+  <si>
+    <t>Alba</t>
+  </si>
+  <si>
+    <t>Derici</t>
+  </si>
+  <si>
+    <t>Sangu</t>
+  </si>
+  <si>
+    <t>Cepkin</t>
+  </si>
+  <si>
+    <t>Tevetoğlu</t>
+  </si>
+  <si>
+    <t>Johnson</t>
+  </si>
+  <si>
+    <t>Sy</t>
+  </si>
+  <si>
+    <t>Evans</t>
+  </si>
+  <si>
+    <t>Winslet</t>
+  </si>
+  <si>
+    <t>Sandler</t>
+  </si>
+  <si>
+    <t>Erçel</t>
+  </si>
+  <si>
+    <t>Scott</t>
+  </si>
+  <si>
+    <t>Riddle</t>
+  </si>
+  <si>
+    <t>Lestrange</t>
+  </si>
+  <si>
+    <t>Chappelle</t>
+  </si>
+  <si>
+    <t>Norton</t>
+  </si>
+  <si>
+    <t>Stark</t>
+  </si>
+  <si>
+    <t>Avşar</t>
+  </si>
+  <si>
+    <t>Schrute</t>
+  </si>
+  <si>
+    <t>Clooney</t>
+  </si>
+  <si>
+    <t>Carrey</t>
+  </si>
+  <si>
+    <t>Baggins</t>
+  </si>
+  <si>
+    <t>Akalın</t>
+  </si>
+  <si>
+    <t>Boluğur</t>
+  </si>
+  <si>
+    <t>Ulusoy</t>
+  </si>
+  <si>
+    <t>Knightley</t>
+  </si>
+  <si>
+    <t>Sert</t>
+  </si>
+  <si>
+    <t>Brown</t>
+  </si>
+  <si>
+    <t>Yılmaz</t>
+  </si>
+  <si>
+    <t>Portman</t>
+  </si>
+  <si>
+    <t>Chan</t>
+  </si>
+  <si>
+    <t>Evcen</t>
+  </si>
+  <si>
+    <t>Timberlake</t>
+  </si>
+  <si>
+    <t>Snow</t>
+  </si>
+  <si>
+    <t>Ziyagil</t>
+  </si>
+  <si>
+    <t>Seinfeld</t>
+  </si>
+  <si>
+    <t>Boz</t>
+  </si>
+  <si>
+    <t>Brando</t>
+  </si>
+  <si>
+    <t>de Armas</t>
+  </si>
+  <si>
+    <t>Dumbledore</t>
+  </si>
+  <si>
+    <t>Kuneri</t>
+  </si>
+  <si>
+    <t>Hiddleston</t>
+  </si>
+  <si>
+    <t>Dalkılıç</t>
+  </si>
+  <si>
+    <t>Özçivit</t>
+  </si>
+  <si>
+    <t>Patient_Priority</t>
+  </si>
+  <si>
+    <t>Operation_Day</t>
+  </si>
   <si>
     <t>Room_No</t>
   </si>
@@ -4573,28 +5698,28 @@
   <sheetData>
     <row r="1">
       <c r="A1" s="0" t="s">
-        <v>1125</v>
+        <v>1500</v>
       </c>
       <c r="B1" s="0" t="s">
-        <v>1126</v>
+        <v>1501</v>
       </c>
       <c r="C1" s="0" t="s">
-        <v>1218</v>
+        <v>1593</v>
       </c>
       <c r="D1" s="0" t="s">
-        <v>1219</v>
+        <v>1594</v>
       </c>
       <c r="E1" s="0" t="s">
-        <v>1312</v>
+        <v>1687</v>
       </c>
       <c r="F1" s="0" t="s">
-        <v>1405</v>
+        <v>1780</v>
       </c>
       <c r="G1" s="0" t="s">
-        <v>1498</v>
+        <v>1873</v>
       </c>
       <c r="H1" s="0" t="s">
-        <v>1499</v>
+        <v>1874</v>
       </c>
     </row>
     <row r="2">
@@ -4602,19 +5727,19 @@
         <v>1</v>
       </c>
       <c r="B2" s="0" t="s">
-        <v>1127</v>
+        <v>1502</v>
       </c>
       <c r="C2" s="0">
         <v>40</v>
       </c>
       <c r="D2" s="0" t="s">
-        <v>1220</v>
+        <v>1595</v>
       </c>
       <c r="E2" s="0" t="s">
-        <v>1313</v>
+        <v>1688</v>
       </c>
       <c r="F2" s="0" t="s">
-        <v>1406</v>
+        <v>1781</v>
       </c>
       <c r="G2" s="0">
         <v>2</v>
@@ -4628,19 +5753,19 @@
         <v>1</v>
       </c>
       <c r="B3" s="0" t="s">
-        <v>1128</v>
+        <v>1503</v>
       </c>
       <c r="C3" s="0">
         <v>80</v>
       </c>
       <c r="D3" s="0" t="s">
-        <v>1221</v>
+        <v>1596</v>
       </c>
       <c r="E3" s="0" t="s">
-        <v>1314</v>
+        <v>1689</v>
       </c>
       <c r="F3" s="0" t="s">
-        <v>1407</v>
+        <v>1782</v>
       </c>
       <c r="G3" s="0">
         <v>1</v>
@@ -4654,19 +5779,19 @@
         <v>1</v>
       </c>
       <c r="B4" s="0" t="s">
-        <v>1129</v>
+        <v>1504</v>
       </c>
       <c r="C4" s="0">
         <v>100</v>
       </c>
       <c r="D4" s="0" t="s">
-        <v>1222</v>
+        <v>1597</v>
       </c>
       <c r="E4" s="0" t="s">
-        <v>1315</v>
+        <v>1690</v>
       </c>
       <c r="F4" s="0" t="s">
-        <v>1408</v>
+        <v>1783</v>
       </c>
       <c r="G4" s="0">
         <v>1</v>
@@ -4680,19 +5805,19 @@
         <v>1</v>
       </c>
       <c r="B5" s="0" t="s">
-        <v>1130</v>
+        <v>1505</v>
       </c>
       <c r="C5" s="0">
         <v>120</v>
       </c>
       <c r="D5" s="0" t="s">
-        <v>1223</v>
+        <v>1598</v>
       </c>
       <c r="E5" s="0" t="s">
-        <v>1316</v>
+        <v>1691</v>
       </c>
       <c r="F5" s="0" t="s">
-        <v>1409</v>
+        <v>1784</v>
       </c>
       <c r="G5" s="0">
         <v>3</v>
@@ -4706,19 +5831,19 @@
         <v>1</v>
       </c>
       <c r="B6" s="0" t="s">
-        <v>1131</v>
+        <v>1506</v>
       </c>
       <c r="C6" s="0">
         <v>80</v>
       </c>
       <c r="D6" s="0" t="s">
-        <v>1224</v>
+        <v>1599</v>
       </c>
       <c r="E6" s="0" t="s">
-        <v>1317</v>
+        <v>1692</v>
       </c>
       <c r="F6" s="0" t="s">
-        <v>1410</v>
+        <v>1785</v>
       </c>
       <c r="G6" s="0">
         <v>2</v>
@@ -4732,19 +5857,19 @@
         <v>1</v>
       </c>
       <c r="B7" s="0" t="s">
-        <v>1132</v>
+        <v>1507</v>
       </c>
       <c r="C7" s="0">
         <v>40</v>
       </c>
       <c r="D7" s="0" t="s">
-        <v>1225</v>
+        <v>1600</v>
       </c>
       <c r="E7" s="0" t="s">
-        <v>1318</v>
+        <v>1693</v>
       </c>
       <c r="F7" s="0" t="s">
-        <v>1411</v>
+        <v>1786</v>
       </c>
       <c r="G7" s="0">
         <v>1</v>
@@ -4758,19 +5883,19 @@
         <v>2</v>
       </c>
       <c r="B8" s="0" t="s">
-        <v>1133</v>
+        <v>1508</v>
       </c>
       <c r="C8" s="0">
         <v>80</v>
       </c>
       <c r="D8" s="0" t="s">
-        <v>1226</v>
+        <v>1601</v>
       </c>
       <c r="E8" s="0" t="s">
-        <v>1319</v>
+        <v>1694</v>
       </c>
       <c r="F8" s="0" t="s">
-        <v>1412</v>
+        <v>1787</v>
       </c>
       <c r="G8" s="0">
         <v>4</v>
@@ -4784,19 +5909,19 @@
         <v>2</v>
       </c>
       <c r="B9" s="0" t="s">
-        <v>1134</v>
+        <v>1509</v>
       </c>
       <c r="C9" s="0">
         <v>60</v>
       </c>
       <c r="D9" s="0" t="s">
-        <v>1227</v>
+        <v>1602</v>
       </c>
       <c r="E9" s="0" t="s">
-        <v>1320</v>
+        <v>1695</v>
       </c>
       <c r="F9" s="0" t="s">
-        <v>1413</v>
+        <v>1788</v>
       </c>
       <c r="G9" s="0">
         <v>1</v>
@@ -4810,19 +5935,19 @@
         <v>2</v>
       </c>
       <c r="B10" s="0" t="s">
-        <v>1135</v>
+        <v>1510</v>
       </c>
       <c r="C10" s="0">
         <v>100</v>
       </c>
       <c r="D10" s="0" t="s">
-        <v>1228</v>
+        <v>1603</v>
       </c>
       <c r="E10" s="0" t="s">
-        <v>1321</v>
+        <v>1696</v>
       </c>
       <c r="F10" s="0" t="s">
-        <v>1414</v>
+        <v>1789</v>
       </c>
       <c r="G10" s="0">
         <v>1</v>
@@ -4836,19 +5961,19 @@
         <v>2</v>
       </c>
       <c r="B11" s="0" t="s">
-        <v>1136</v>
+        <v>1511</v>
       </c>
       <c r="C11" s="0">
         <v>60</v>
       </c>
       <c r="D11" s="0" t="s">
-        <v>1229</v>
+        <v>1604</v>
       </c>
       <c r="E11" s="0" t="s">
-        <v>1322</v>
+        <v>1697</v>
       </c>
       <c r="F11" s="0" t="s">
-        <v>1415</v>
+        <v>1790</v>
       </c>
       <c r="G11" s="0">
         <v>1</v>
@@ -4862,19 +5987,19 @@
         <v>2</v>
       </c>
       <c r="B12" s="0" t="s">
-        <v>1137</v>
+        <v>1512</v>
       </c>
       <c r="C12" s="0">
         <v>80</v>
       </c>
       <c r="D12" s="0" t="s">
-        <v>1230</v>
+        <v>1605</v>
       </c>
       <c r="E12" s="0" t="s">
-        <v>1323</v>
+        <v>1698</v>
       </c>
       <c r="F12" s="0" t="s">
-        <v>1416</v>
+        <v>1791</v>
       </c>
       <c r="G12" s="0">
         <v>2</v>
@@ -4888,19 +6013,19 @@
         <v>2</v>
       </c>
       <c r="B13" s="0" t="s">
-        <v>1138</v>
+        <v>1513</v>
       </c>
       <c r="C13" s="0">
         <v>80</v>
       </c>
       <c r="D13" s="0" t="s">
-        <v>1231</v>
+        <v>1606</v>
       </c>
       <c r="E13" s="0" t="s">
-        <v>1324</v>
+        <v>1699</v>
       </c>
       <c r="F13" s="0" t="s">
-        <v>1417</v>
+        <v>1792</v>
       </c>
       <c r="G13" s="0">
         <v>2</v>
@@ -4914,19 +6039,19 @@
         <v>3</v>
       </c>
       <c r="B14" s="0" t="s">
-        <v>1139</v>
+        <v>1514</v>
       </c>
       <c r="C14" s="0">
         <v>20</v>
       </c>
       <c r="D14" s="0" t="s">
-        <v>1232</v>
+        <v>1607</v>
       </c>
       <c r="E14" s="0" t="s">
-        <v>1325</v>
+        <v>1700</v>
       </c>
       <c r="F14" s="0" t="s">
-        <v>1418</v>
+        <v>1793</v>
       </c>
       <c r="G14" s="0">
         <v>2</v>
@@ -4940,19 +6065,19 @@
         <v>3</v>
       </c>
       <c r="B15" s="0" t="s">
-        <v>1140</v>
+        <v>1515</v>
       </c>
       <c r="C15" s="0">
         <v>60</v>
       </c>
       <c r="D15" s="0" t="s">
-        <v>1233</v>
+        <v>1608</v>
       </c>
       <c r="E15" s="0" t="s">
-        <v>1326</v>
+        <v>1701</v>
       </c>
       <c r="F15" s="0" t="s">
-        <v>1419</v>
+        <v>1794</v>
       </c>
       <c r="G15" s="0">
         <v>2</v>
@@ -4966,19 +6091,19 @@
         <v>3</v>
       </c>
       <c r="B16" s="0" t="s">
-        <v>1141</v>
+        <v>1516</v>
       </c>
       <c r="C16" s="0">
         <v>40</v>
       </c>
       <c r="D16" s="0" t="s">
-        <v>1234</v>
+        <v>1609</v>
       </c>
       <c r="E16" s="0" t="s">
-        <v>1327</v>
+        <v>1702</v>
       </c>
       <c r="F16" s="0" t="s">
-        <v>1420</v>
+        <v>1795</v>
       </c>
       <c r="G16" s="0">
         <v>2</v>
@@ -4992,19 +6117,19 @@
         <v>3</v>
       </c>
       <c r="B17" s="0" t="s">
-        <v>1142</v>
+        <v>1517</v>
       </c>
       <c r="C17" s="0">
         <v>60</v>
       </c>
       <c r="D17" s="0" t="s">
-        <v>1235</v>
+        <v>1610</v>
       </c>
       <c r="E17" s="0" t="s">
-        <v>1328</v>
+        <v>1703</v>
       </c>
       <c r="F17" s="0" t="s">
-        <v>1421</v>
+        <v>1796</v>
       </c>
       <c r="G17" s="0">
         <v>3</v>
@@ -5018,19 +6143,19 @@
         <v>3</v>
       </c>
       <c r="B18" s="0" t="s">
-        <v>1143</v>
+        <v>1518</v>
       </c>
       <c r="C18" s="0">
         <v>40</v>
       </c>
       <c r="D18" s="0" t="s">
-        <v>1236</v>
+        <v>1611</v>
       </c>
       <c r="E18" s="0" t="s">
-        <v>1329</v>
+        <v>1704</v>
       </c>
       <c r="F18" s="0" t="s">
-        <v>1422</v>
+        <v>1797</v>
       </c>
       <c r="G18" s="0">
         <v>4</v>
@@ -5044,19 +6169,19 @@
         <v>3</v>
       </c>
       <c r="B19" s="0" t="s">
-        <v>1144</v>
+        <v>1519</v>
       </c>
       <c r="C19" s="0">
         <v>40</v>
       </c>
       <c r="D19" s="0" t="s">
-        <v>1237</v>
+        <v>1612</v>
       </c>
       <c r="E19" s="0" t="s">
-        <v>1330</v>
+        <v>1705</v>
       </c>
       <c r="F19" s="0" t="s">
-        <v>1423</v>
+        <v>1798</v>
       </c>
       <c r="G19" s="0">
         <v>2</v>
@@ -5070,19 +6195,19 @@
         <v>3</v>
       </c>
       <c r="B20" s="0" t="s">
-        <v>1145</v>
+        <v>1520</v>
       </c>
       <c r="C20" s="0">
         <v>80</v>
       </c>
       <c r="D20" s="0" t="s">
-        <v>1238</v>
+        <v>1613</v>
       </c>
       <c r="E20" s="0" t="s">
-        <v>1331</v>
+        <v>1706</v>
       </c>
       <c r="F20" s="0" t="s">
-        <v>1424</v>
+        <v>1799</v>
       </c>
       <c r="G20" s="0">
         <v>2</v>
@@ -5096,19 +6221,19 @@
         <v>1</v>
       </c>
       <c r="B21" s="0" t="s">
-        <v>1146</v>
+        <v>1521</v>
       </c>
       <c r="C21" s="0">
         <v>20</v>
       </c>
       <c r="D21" s="0" t="s">
-        <v>1239</v>
+        <v>1614</v>
       </c>
       <c r="E21" s="0" t="s">
-        <v>1332</v>
+        <v>1707</v>
       </c>
       <c r="F21" s="0" t="s">
-        <v>1425</v>
+        <v>1800</v>
       </c>
       <c r="G21" s="0">
         <v>0</v>
@@ -5122,19 +6247,19 @@
         <v>1</v>
       </c>
       <c r="B22" s="0" t="s">
-        <v>1147</v>
+        <v>1522</v>
       </c>
       <c r="C22" s="0">
         <v>120</v>
       </c>
       <c r="D22" s="0" t="s">
-        <v>1240</v>
+        <v>1615</v>
       </c>
       <c r="E22" s="0" t="s">
-        <v>1333</v>
+        <v>1708</v>
       </c>
       <c r="F22" s="0" t="s">
-        <v>1426</v>
+        <v>1801</v>
       </c>
       <c r="G22" s="0">
         <v>1</v>
@@ -5148,19 +6273,19 @@
         <v>1</v>
       </c>
       <c r="B23" s="0" t="s">
-        <v>1148</v>
+        <v>1523</v>
       </c>
       <c r="C23" s="0">
         <v>120</v>
       </c>
       <c r="D23" s="0" t="s">
-        <v>1241</v>
+        <v>1616</v>
       </c>
       <c r="E23" s="0" t="s">
-        <v>1334</v>
+        <v>1709</v>
       </c>
       <c r="F23" s="0" t="s">
-        <v>1427</v>
+        <v>1802</v>
       </c>
       <c r="G23" s="0">
         <v>2</v>
@@ -5174,19 +6299,19 @@
         <v>1</v>
       </c>
       <c r="B24" s="0" t="s">
-        <v>1149</v>
+        <v>1524</v>
       </c>
       <c r="C24" s="0">
         <v>40</v>
       </c>
       <c r="D24" s="0" t="s">
-        <v>1242</v>
+        <v>1617</v>
       </c>
       <c r="E24" s="0" t="s">
-        <v>1335</v>
+        <v>1710</v>
       </c>
       <c r="F24" s="0" t="s">
-        <v>1428</v>
+        <v>1803</v>
       </c>
       <c r="G24" s="0">
         <v>2</v>
@@ -5200,19 +6325,19 @@
         <v>1</v>
       </c>
       <c r="B25" s="0" t="s">
-        <v>1150</v>
+        <v>1525</v>
       </c>
       <c r="C25" s="0">
         <v>60</v>
       </c>
       <c r="D25" s="0" t="s">
-        <v>1243</v>
+        <v>1618</v>
       </c>
       <c r="E25" s="0" t="s">
-        <v>1336</v>
+        <v>1711</v>
       </c>
       <c r="F25" s="0" t="s">
-        <v>1429</v>
+        <v>1804</v>
       </c>
       <c r="G25" s="0">
         <v>1</v>
@@ -5226,19 +6351,19 @@
         <v>1</v>
       </c>
       <c r="B26" s="0" t="s">
-        <v>1151</v>
+        <v>1526</v>
       </c>
       <c r="C26" s="0">
         <v>100</v>
       </c>
       <c r="D26" s="0" t="s">
-        <v>1244</v>
+        <v>1619</v>
       </c>
       <c r="E26" s="0" t="s">
-        <v>1337</v>
+        <v>1712</v>
       </c>
       <c r="F26" s="0" t="s">
-        <v>1430</v>
+        <v>1805</v>
       </c>
       <c r="G26" s="0">
         <v>1</v>
@@ -5252,19 +6377,19 @@
         <v>2</v>
       </c>
       <c r="B27" s="0" t="s">
-        <v>1152</v>
+        <v>1527</v>
       </c>
       <c r="C27" s="0">
         <v>120</v>
       </c>
       <c r="D27" s="0" t="s">
-        <v>1245</v>
+        <v>1620</v>
       </c>
       <c r="E27" s="0" t="s">
-        <v>1338</v>
+        <v>1713</v>
       </c>
       <c r="F27" s="0" t="s">
-        <v>1431</v>
+        <v>1806</v>
       </c>
       <c r="G27" s="0">
         <v>1</v>
@@ -5278,19 +6403,19 @@
         <v>2</v>
       </c>
       <c r="B28" s="0" t="s">
-        <v>1153</v>
+        <v>1528</v>
       </c>
       <c r="C28" s="0">
         <v>100</v>
       </c>
       <c r="D28" s="0" t="s">
-        <v>1246</v>
+        <v>1621</v>
       </c>
       <c r="E28" s="0" t="s">
-        <v>1339</v>
+        <v>1714</v>
       </c>
       <c r="F28" s="0" t="s">
-        <v>1432</v>
+        <v>1807</v>
       </c>
       <c r="G28" s="0">
         <v>4</v>
@@ -5304,19 +6429,19 @@
         <v>2</v>
       </c>
       <c r="B29" s="0" t="s">
-        <v>1154</v>
+        <v>1529</v>
       </c>
       <c r="C29" s="0">
         <v>60</v>
       </c>
       <c r="D29" s="0" t="s">
-        <v>1247</v>
+        <v>1622</v>
       </c>
       <c r="E29" s="0" t="s">
-        <v>1340</v>
+        <v>1715</v>
       </c>
       <c r="F29" s="0" t="s">
-        <v>1433</v>
+        <v>1808</v>
       </c>
       <c r="G29" s="0">
         <v>2</v>
@@ -5330,19 +6455,19 @@
         <v>2</v>
       </c>
       <c r="B30" s="0" t="s">
-        <v>1155</v>
+        <v>1530</v>
       </c>
       <c r="C30" s="0">
         <v>20</v>
       </c>
       <c r="D30" s="0" t="s">
-        <v>1248</v>
+        <v>1623</v>
       </c>
       <c r="E30" s="0" t="s">
-        <v>1341</v>
+        <v>1716</v>
       </c>
       <c r="F30" s="0" t="s">
-        <v>1434</v>
+        <v>1809</v>
       </c>
       <c r="G30" s="0">
         <v>1</v>
@@ -5356,19 +6481,19 @@
         <v>2</v>
       </c>
       <c r="B31" s="0" t="s">
-        <v>1156</v>
+        <v>1531</v>
       </c>
       <c r="C31" s="0">
         <v>120</v>
       </c>
       <c r="D31" s="0" t="s">
-        <v>1249</v>
+        <v>1624</v>
       </c>
       <c r="E31" s="0" t="s">
-        <v>1342</v>
+        <v>1717</v>
       </c>
       <c r="F31" s="0" t="s">
-        <v>1435</v>
+        <v>1810</v>
       </c>
       <c r="G31" s="0">
         <v>4</v>
@@ -5382,19 +6507,19 @@
         <v>3</v>
       </c>
       <c r="B32" s="0" t="s">
-        <v>1157</v>
+        <v>1532</v>
       </c>
       <c r="C32" s="0">
         <v>20</v>
       </c>
       <c r="D32" s="0" t="s">
-        <v>1250</v>
+        <v>1625</v>
       </c>
       <c r="E32" s="0" t="s">
-        <v>1343</v>
+        <v>1718</v>
       </c>
       <c r="F32" s="0" t="s">
-        <v>1436</v>
+        <v>1811</v>
       </c>
       <c r="G32" s="0">
         <v>4</v>
@@ -5408,19 +6533,19 @@
         <v>3</v>
       </c>
       <c r="B33" s="0" t="s">
-        <v>1158</v>
+        <v>1533</v>
       </c>
       <c r="C33" s="0">
         <v>100</v>
       </c>
       <c r="D33" s="0" t="s">
-        <v>1251</v>
+        <v>1626</v>
       </c>
       <c r="E33" s="0" t="s">
-        <v>1344</v>
+        <v>1719</v>
       </c>
       <c r="F33" s="0" t="s">
-        <v>1437</v>
+        <v>1812</v>
       </c>
       <c r="G33" s="0">
         <v>1</v>
@@ -5434,19 +6559,19 @@
         <v>3</v>
       </c>
       <c r="B34" s="0" t="s">
-        <v>1159</v>
+        <v>1534</v>
       </c>
       <c r="C34" s="0">
         <v>40</v>
       </c>
       <c r="D34" s="0" t="s">
-        <v>1252</v>
+        <v>1627</v>
       </c>
       <c r="E34" s="0" t="s">
-        <v>1345</v>
+        <v>1720</v>
       </c>
       <c r="F34" s="0" t="s">
-        <v>1438</v>
+        <v>1813</v>
       </c>
       <c r="G34" s="0">
         <v>2</v>
@@ -5460,19 +6585,19 @@
         <v>3</v>
       </c>
       <c r="B35" s="0" t="s">
-        <v>1160</v>
+        <v>1535</v>
       </c>
       <c r="C35" s="0">
         <v>20</v>
       </c>
       <c r="D35" s="0" t="s">
-        <v>1253</v>
+        <v>1628</v>
       </c>
       <c r="E35" s="0" t="s">
-        <v>1346</v>
+        <v>1721</v>
       </c>
       <c r="F35" s="0" t="s">
-        <v>1439</v>
+        <v>1814</v>
       </c>
       <c r="G35" s="0">
         <v>4</v>
@@ -5486,19 +6611,19 @@
         <v>3</v>
       </c>
       <c r="B36" s="0" t="s">
-        <v>1161</v>
+        <v>1536</v>
       </c>
       <c r="C36" s="0">
         <v>40</v>
       </c>
       <c r="D36" s="0" t="s">
-        <v>1254</v>
+        <v>1629</v>
       </c>
       <c r="E36" s="0" t="s">
-        <v>1347</v>
+        <v>1722</v>
       </c>
       <c r="F36" s="0" t="s">
-        <v>1440</v>
+        <v>1815</v>
       </c>
       <c r="G36" s="0">
         <v>2</v>
@@ -5512,19 +6637,19 @@
         <v>3</v>
       </c>
       <c r="B37" s="0" t="s">
-        <v>1162</v>
+        <v>1537</v>
       </c>
       <c r="C37" s="0">
         <v>80</v>
       </c>
       <c r="D37" s="0" t="s">
-        <v>1255</v>
+        <v>1630</v>
       </c>
       <c r="E37" s="0" t="s">
-        <v>1348</v>
+        <v>1723</v>
       </c>
       <c r="F37" s="0" t="s">
-        <v>1441</v>
+        <v>1816</v>
       </c>
       <c r="G37" s="0">
         <v>4</v>
@@ -5538,19 +6663,19 @@
         <v>1</v>
       </c>
       <c r="B38" s="0" t="s">
-        <v>1163</v>
+        <v>1538</v>
       </c>
       <c r="C38" s="0">
         <v>120</v>
       </c>
       <c r="D38" s="0" t="s">
-        <v>1256</v>
+        <v>1631</v>
       </c>
       <c r="E38" s="0" t="s">
-        <v>1349</v>
+        <v>1724</v>
       </c>
       <c r="F38" s="0" t="s">
-        <v>1442</v>
+        <v>1817</v>
       </c>
       <c r="G38" s="0">
         <v>0</v>
@@ -5564,19 +6689,19 @@
         <v>1</v>
       </c>
       <c r="B39" s="0" t="s">
-        <v>1164</v>
+        <v>1539</v>
       </c>
       <c r="C39" s="0">
         <v>100</v>
       </c>
       <c r="D39" s="0" t="s">
-        <v>1257</v>
+        <v>1632</v>
       </c>
       <c r="E39" s="0" t="s">
-        <v>1350</v>
+        <v>1725</v>
       </c>
       <c r="F39" s="0" t="s">
-        <v>1443</v>
+        <v>1818</v>
       </c>
       <c r="G39" s="0">
         <v>1</v>
@@ -5590,19 +6715,19 @@
         <v>1</v>
       </c>
       <c r="B40" s="0" t="s">
-        <v>1165</v>
+        <v>1540</v>
       </c>
       <c r="C40" s="0">
         <v>20</v>
       </c>
       <c r="D40" s="0" t="s">
-        <v>1258</v>
+        <v>1633</v>
       </c>
       <c r="E40" s="0" t="s">
-        <v>1351</v>
+        <v>1726</v>
       </c>
       <c r="F40" s="0" t="s">
-        <v>1444</v>
+        <v>1819</v>
       </c>
       <c r="G40" s="0">
         <v>4</v>
@@ -5616,19 +6741,19 @@
         <v>1</v>
       </c>
       <c r="B41" s="0" t="s">
-        <v>1166</v>
+        <v>1541</v>
       </c>
       <c r="C41" s="0">
         <v>100</v>
       </c>
       <c r="D41" s="0" t="s">
-        <v>1259</v>
+        <v>1634</v>
       </c>
       <c r="E41" s="0" t="s">
-        <v>1352</v>
+        <v>1727</v>
       </c>
       <c r="F41" s="0" t="s">
-        <v>1445</v>
+        <v>1820</v>
       </c>
       <c r="G41" s="0">
         <v>1</v>
@@ -5642,19 +6767,19 @@
         <v>1</v>
       </c>
       <c r="B42" s="0" t="s">
-        <v>1167</v>
+        <v>1542</v>
       </c>
       <c r="C42" s="0">
         <v>20</v>
       </c>
       <c r="D42" s="0" t="s">
-        <v>1260</v>
+        <v>1635</v>
       </c>
       <c r="E42" s="0" t="s">
-        <v>1353</v>
+        <v>1728</v>
       </c>
       <c r="F42" s="0" t="s">
-        <v>1446</v>
+        <v>1821</v>
       </c>
       <c r="G42" s="0">
         <v>1</v>
@@ -5668,19 +6793,19 @@
         <v>1</v>
       </c>
       <c r="B43" s="0" t="s">
-        <v>1168</v>
+        <v>1543</v>
       </c>
       <c r="C43" s="0">
         <v>120</v>
       </c>
       <c r="D43" s="0" t="s">
-        <v>1261</v>
+        <v>1636</v>
       </c>
       <c r="E43" s="0" t="s">
-        <v>1354</v>
+        <v>1729</v>
       </c>
       <c r="F43" s="0" t="s">
-        <v>1447</v>
+        <v>1822</v>
       </c>
       <c r="G43" s="0">
         <v>2</v>
@@ -5694,19 +6819,19 @@
         <v>2</v>
       </c>
       <c r="B44" s="0" t="s">
-        <v>1169</v>
+        <v>1544</v>
       </c>
       <c r="C44" s="0">
         <v>40</v>
       </c>
       <c r="D44" s="0" t="s">
-        <v>1262</v>
+        <v>1637</v>
       </c>
       <c r="E44" s="0" t="s">
-        <v>1355</v>
+        <v>1730</v>
       </c>
       <c r="F44" s="0" t="s">
-        <v>1448</v>
+        <v>1823</v>
       </c>
       <c r="G44" s="0">
         <v>0</v>
@@ -5720,19 +6845,19 @@
         <v>2</v>
       </c>
       <c r="B45" s="0" t="s">
-        <v>1170</v>
+        <v>1545</v>
       </c>
       <c r="C45" s="0">
         <v>20</v>
       </c>
       <c r="D45" s="0" t="s">
-        <v>1263</v>
+        <v>1638</v>
       </c>
       <c r="E45" s="0" t="s">
-        <v>1356</v>
+        <v>1731</v>
       </c>
       <c r="F45" s="0" t="s">
-        <v>1449</v>
+        <v>1824</v>
       </c>
       <c r="G45" s="0">
         <v>1</v>
@@ -5746,19 +6871,19 @@
         <v>2</v>
       </c>
       <c r="B46" s="0" t="s">
-        <v>1171</v>
+        <v>1546</v>
       </c>
       <c r="C46" s="0">
         <v>100</v>
       </c>
       <c r="D46" s="0" t="s">
-        <v>1264</v>
+        <v>1639</v>
       </c>
       <c r="E46" s="0" t="s">
-        <v>1357</v>
+        <v>1732</v>
       </c>
       <c r="F46" s="0" t="s">
-        <v>1450</v>
+        <v>1825</v>
       </c>
       <c r="G46" s="0">
         <v>2</v>
@@ -5772,19 +6897,19 @@
         <v>2</v>
       </c>
       <c r="B47" s="0" t="s">
-        <v>1172</v>
+        <v>1547</v>
       </c>
       <c r="C47" s="0">
         <v>20</v>
       </c>
       <c r="D47" s="0" t="s">
-        <v>1265</v>
+        <v>1640</v>
       </c>
       <c r="E47" s="0" t="s">
-        <v>1358</v>
+        <v>1733</v>
       </c>
       <c r="F47" s="0" t="s">
-        <v>1451</v>
+        <v>1826</v>
       </c>
       <c r="G47" s="0">
         <v>1</v>
@@ -5798,19 +6923,19 @@
         <v>2</v>
       </c>
       <c r="B48" s="0" t="s">
-        <v>1173</v>
+        <v>1548</v>
       </c>
       <c r="C48" s="0">
         <v>100</v>
       </c>
       <c r="D48" s="0" t="s">
-        <v>1266</v>
+        <v>1641</v>
       </c>
       <c r="E48" s="0" t="s">
-        <v>1359</v>
+        <v>1734</v>
       </c>
       <c r="F48" s="0" t="s">
-        <v>1452</v>
+        <v>1827</v>
       </c>
       <c r="G48" s="0">
         <v>2</v>
@@ -5824,19 +6949,19 @@
         <v>2</v>
       </c>
       <c r="B49" s="0" t="s">
-        <v>1174</v>
+        <v>1549</v>
       </c>
       <c r="C49" s="0">
         <v>60</v>
       </c>
       <c r="D49" s="0" t="s">
-        <v>1267</v>
+        <v>1642</v>
       </c>
       <c r="E49" s="0" t="s">
-        <v>1360</v>
+        <v>1735</v>
       </c>
       <c r="F49" s="0" t="s">
-        <v>1453</v>
+        <v>1828</v>
       </c>
       <c r="G49" s="0">
         <v>3</v>
@@ -5850,19 +6975,19 @@
         <v>3</v>
       </c>
       <c r="B50" s="0" t="s">
-        <v>1175</v>
+        <v>1550</v>
       </c>
       <c r="C50" s="0">
         <v>60</v>
       </c>
       <c r="D50" s="0" t="s">
-        <v>1268</v>
+        <v>1643</v>
       </c>
       <c r="E50" s="0" t="s">
-        <v>1361</v>
+        <v>1736</v>
       </c>
       <c r="F50" s="0" t="s">
-        <v>1454</v>
+        <v>1829</v>
       </c>
       <c r="G50" s="0">
         <v>0</v>
@@ -5876,19 +7001,19 @@
         <v>3</v>
       </c>
       <c r="B51" s="0" t="s">
-        <v>1176</v>
+        <v>1551</v>
       </c>
       <c r="C51" s="0">
         <v>20</v>
       </c>
       <c r="D51" s="0" t="s">
-        <v>1269</v>
+        <v>1644</v>
       </c>
       <c r="E51" s="0" t="s">
-        <v>1362</v>
+        <v>1737</v>
       </c>
       <c r="F51" s="0" t="s">
-        <v>1455</v>
+        <v>1830</v>
       </c>
       <c r="G51" s="0">
         <v>3</v>
@@ -5902,19 +7027,19 @@
         <v>3</v>
       </c>
       <c r="B52" s="0" t="s">
-        <v>1177</v>
+        <v>1552</v>
       </c>
       <c r="C52" s="0">
         <v>20</v>
       </c>
       <c r="D52" s="0" t="s">
-        <v>1270</v>
+        <v>1645</v>
       </c>
       <c r="E52" s="0" t="s">
-        <v>1363</v>
+        <v>1738</v>
       </c>
       <c r="F52" s="0" t="s">
-        <v>1456</v>
+        <v>1831</v>
       </c>
       <c r="G52" s="0">
         <v>4</v>
@@ -5928,19 +7053,19 @@
         <v>3</v>
       </c>
       <c r="B53" s="0" t="s">
-        <v>1178</v>
+        <v>1553</v>
       </c>
       <c r="C53" s="0">
         <v>20</v>
       </c>
       <c r="D53" s="0" t="s">
-        <v>1271</v>
+        <v>1646</v>
       </c>
       <c r="E53" s="0" t="s">
-        <v>1364</v>
+        <v>1739</v>
       </c>
       <c r="F53" s="0" t="s">
-        <v>1457</v>
+        <v>1832</v>
       </c>
       <c r="G53" s="0">
         <v>4</v>
@@ -5954,19 +7079,19 @@
         <v>3</v>
       </c>
       <c r="B54" s="0" t="s">
-        <v>1179</v>
+        <v>1554</v>
       </c>
       <c r="C54" s="0">
         <v>100</v>
       </c>
       <c r="D54" s="0" t="s">
-        <v>1272</v>
+        <v>1647</v>
       </c>
       <c r="E54" s="0" t="s">
-        <v>1365</v>
+        <v>1740</v>
       </c>
       <c r="F54" s="0" t="s">
-        <v>1458</v>
+        <v>1833</v>
       </c>
       <c r="G54" s="0">
         <v>1</v>
@@ -5980,19 +7105,19 @@
         <v>3</v>
       </c>
       <c r="B55" s="0" t="s">
-        <v>1180</v>
+        <v>1555</v>
       </c>
       <c r="C55" s="0">
         <v>20</v>
       </c>
       <c r="D55" s="0" t="s">
-        <v>1273</v>
+        <v>1648</v>
       </c>
       <c r="E55" s="0" t="s">
-        <v>1366</v>
+        <v>1741</v>
       </c>
       <c r="F55" s="0" t="s">
-        <v>1459</v>
+        <v>1834</v>
       </c>
       <c r="G55" s="0">
         <v>3</v>
@@ -6006,19 +7131,19 @@
         <v>3</v>
       </c>
       <c r="B56" s="0" t="s">
-        <v>1181</v>
+        <v>1556</v>
       </c>
       <c r="C56" s="0">
         <v>120</v>
       </c>
       <c r="D56" s="0" t="s">
-        <v>1274</v>
+        <v>1649</v>
       </c>
       <c r="E56" s="0" t="s">
-        <v>1367</v>
+        <v>1742</v>
       </c>
       <c r="F56" s="0" t="s">
-        <v>1460</v>
+        <v>1835</v>
       </c>
       <c r="G56" s="0">
         <v>3</v>
@@ -6032,19 +7157,19 @@
         <v>1</v>
       </c>
       <c r="B57" s="0" t="s">
-        <v>1182</v>
+        <v>1557</v>
       </c>
       <c r="C57" s="0">
         <v>60</v>
       </c>
       <c r="D57" s="0" t="s">
-        <v>1275</v>
+        <v>1650</v>
       </c>
       <c r="E57" s="0" t="s">
-        <v>1368</v>
+        <v>1743</v>
       </c>
       <c r="F57" s="0" t="s">
-        <v>1461</v>
+        <v>1836</v>
       </c>
       <c r="G57" s="0">
         <v>0</v>
@@ -6058,19 +7183,19 @@
         <v>1</v>
       </c>
       <c r="B58" s="0" t="s">
-        <v>1183</v>
+        <v>1558</v>
       </c>
       <c r="C58" s="0">
         <v>20</v>
       </c>
       <c r="D58" s="0" t="s">
-        <v>1276</v>
+        <v>1651</v>
       </c>
       <c r="E58" s="0" t="s">
-        <v>1369</v>
+        <v>1744</v>
       </c>
       <c r="F58" s="0" t="s">
-        <v>1462</v>
+        <v>1837</v>
       </c>
       <c r="G58" s="0">
         <v>1</v>
@@ -6084,19 +7209,19 @@
         <v>1</v>
       </c>
       <c r="B59" s="0" t="s">
-        <v>1183</v>
+        <v>1558</v>
       </c>
       <c r="C59" s="0">
         <v>20</v>
       </c>
       <c r="D59" s="0" t="s">
-        <v>1277</v>
+        <v>1652</v>
       </c>
       <c r="E59" s="0" t="s">
-        <v>1370</v>
+        <v>1745</v>
       </c>
       <c r="F59" s="0" t="s">
-        <v>1463</v>
+        <v>1838</v>
       </c>
       <c r="G59" s="0">
         <v>2</v>
@@ -6110,19 +7235,19 @@
         <v>1</v>
       </c>
       <c r="B60" s="0" t="s">
-        <v>1184</v>
+        <v>1559</v>
       </c>
       <c r="C60" s="0">
         <v>40</v>
       </c>
       <c r="D60" s="0" t="s">
-        <v>1278</v>
+        <v>1653</v>
       </c>
       <c r="E60" s="0" t="s">
-        <v>1371</v>
+        <v>1746</v>
       </c>
       <c r="F60" s="0" t="s">
-        <v>1464</v>
+        <v>1839</v>
       </c>
       <c r="G60" s="0">
         <v>1</v>
@@ -6136,19 +7261,19 @@
         <v>1</v>
       </c>
       <c r="B61" s="0" t="s">
-        <v>1185</v>
+        <v>1560</v>
       </c>
       <c r="C61" s="0">
         <v>120</v>
       </c>
       <c r="D61" s="0" t="s">
-        <v>1279</v>
+        <v>1654</v>
       </c>
       <c r="E61" s="0" t="s">
-        <v>1372</v>
+        <v>1747</v>
       </c>
       <c r="F61" s="0" t="s">
-        <v>1465</v>
+        <v>1840</v>
       </c>
       <c r="G61" s="0">
         <v>1</v>
@@ -6162,19 +7287,19 @@
         <v>1</v>
       </c>
       <c r="B62" s="0" t="s">
-        <v>1186</v>
+        <v>1561</v>
       </c>
       <c r="C62" s="0">
         <v>100</v>
       </c>
       <c r="D62" s="0" t="s">
-        <v>1280</v>
+        <v>1655</v>
       </c>
       <c r="E62" s="0" t="s">
-        <v>1373</v>
+        <v>1748</v>
       </c>
       <c r="F62" s="0" t="s">
-        <v>1466</v>
+        <v>1841</v>
       </c>
       <c r="G62" s="0">
         <v>3</v>
@@ -6188,19 +7313,19 @@
         <v>1</v>
       </c>
       <c r="B63" s="0" t="s">
-        <v>1187</v>
+        <v>1562</v>
       </c>
       <c r="C63" s="0">
         <v>20</v>
       </c>
       <c r="D63" s="0" t="s">
-        <v>1281</v>
+        <v>1656</v>
       </c>
       <c r="E63" s="0" t="s">
-        <v>1374</v>
+        <v>1749</v>
       </c>
       <c r="F63" s="0" t="s">
-        <v>1467</v>
+        <v>1842</v>
       </c>
       <c r="G63" s="0">
         <v>1</v>
@@ -6214,19 +7339,19 @@
         <v>1</v>
       </c>
       <c r="B64" s="0" t="s">
-        <v>1188</v>
+        <v>1563</v>
       </c>
       <c r="C64" s="0">
         <v>60</v>
       </c>
       <c r="D64" s="0" t="s">
-        <v>1282</v>
+        <v>1657</v>
       </c>
       <c r="E64" s="0" t="s">
-        <v>1375</v>
+        <v>1750</v>
       </c>
       <c r="F64" s="0" t="s">
-        <v>1468</v>
+        <v>1843</v>
       </c>
       <c r="G64" s="0">
         <v>4</v>
@@ -6240,19 +7365,19 @@
         <v>1</v>
       </c>
       <c r="B65" s="0" t="s">
-        <v>1189</v>
+        <v>1564</v>
       </c>
       <c r="C65" s="0">
         <v>20</v>
       </c>
       <c r="D65" s="0" t="s">
-        <v>1283</v>
+        <v>1658</v>
       </c>
       <c r="E65" s="0" t="s">
-        <v>1376</v>
+        <v>1751</v>
       </c>
       <c r="F65" s="0" t="s">
-        <v>1469</v>
+        <v>1844</v>
       </c>
       <c r="G65" s="0">
         <v>2</v>
@@ -6266,19 +7391,19 @@
         <v>2</v>
       </c>
       <c r="B66" s="0" t="s">
-        <v>1190</v>
+        <v>1565</v>
       </c>
       <c r="C66" s="0">
         <v>20</v>
       </c>
       <c r="D66" s="0" t="s">
-        <v>1284</v>
+        <v>1659</v>
       </c>
       <c r="E66" s="0" t="s">
-        <v>1377</v>
+        <v>1752</v>
       </c>
       <c r="F66" s="0" t="s">
-        <v>1470</v>
+        <v>1845</v>
       </c>
       <c r="G66" s="0">
         <v>0</v>
@@ -6292,19 +7417,19 @@
         <v>2</v>
       </c>
       <c r="B67" s="0" t="s">
-        <v>1191</v>
+        <v>1566</v>
       </c>
       <c r="C67" s="0">
         <v>20</v>
       </c>
       <c r="D67" s="0" t="s">
-        <v>1285</v>
+        <v>1660</v>
       </c>
       <c r="E67" s="0" t="s">
-        <v>1378</v>
+        <v>1753</v>
       </c>
       <c r="F67" s="0" t="s">
-        <v>1471</v>
+        <v>1846</v>
       </c>
       <c r="G67" s="0">
         <v>1</v>
@@ -6318,19 +7443,19 @@
         <v>2</v>
       </c>
       <c r="B68" s="0" t="s">
-        <v>1192</v>
+        <v>1567</v>
       </c>
       <c r="C68" s="0">
         <v>60</v>
       </c>
       <c r="D68" s="0" t="s">
-        <v>1286</v>
+        <v>1661</v>
       </c>
       <c r="E68" s="0" t="s">
-        <v>1379</v>
+        <v>1754</v>
       </c>
       <c r="F68" s="0" t="s">
-        <v>1472</v>
+        <v>1847</v>
       </c>
       <c r="G68" s="0">
         <v>2</v>
@@ -6344,19 +7469,19 @@
         <v>2</v>
       </c>
       <c r="B69" s="0" t="s">
-        <v>1193</v>
+        <v>1568</v>
       </c>
       <c r="C69" s="0">
         <v>40</v>
       </c>
       <c r="D69" s="0" t="s">
-        <v>1287</v>
+        <v>1662</v>
       </c>
       <c r="E69" s="0" t="s">
-        <v>1380</v>
+        <v>1755</v>
       </c>
       <c r="F69" s="0" t="s">
-        <v>1473</v>
+        <v>1848</v>
       </c>
       <c r="G69" s="0">
         <v>3</v>
@@ -6370,19 +7495,19 @@
         <v>2</v>
       </c>
       <c r="B70" s="0" t="s">
-        <v>1194</v>
+        <v>1569</v>
       </c>
       <c r="C70" s="0">
         <v>120</v>
       </c>
       <c r="D70" s="0" t="s">
-        <v>1288</v>
+        <v>1663</v>
       </c>
       <c r="E70" s="0" t="s">
-        <v>1381</v>
+        <v>1756</v>
       </c>
       <c r="F70" s="0" t="s">
-        <v>1474</v>
+        <v>1849</v>
       </c>
       <c r="G70" s="0">
         <v>4</v>
@@ -6396,19 +7521,19 @@
         <v>2</v>
       </c>
       <c r="B71" s="0" t="s">
-        <v>1195</v>
+        <v>1570</v>
       </c>
       <c r="C71" s="0">
         <v>20</v>
       </c>
       <c r="D71" s="0" t="s">
-        <v>1289</v>
+        <v>1664</v>
       </c>
       <c r="E71" s="0" t="s">
-        <v>1382</v>
+        <v>1757</v>
       </c>
       <c r="F71" s="0" t="s">
-        <v>1475</v>
+        <v>1850</v>
       </c>
       <c r="G71" s="0">
         <v>3</v>
@@ -6422,19 +7547,19 @@
         <v>2</v>
       </c>
       <c r="B72" s="0" t="s">
-        <v>1196</v>
+        <v>1571</v>
       </c>
       <c r="C72" s="0">
         <v>100</v>
       </c>
       <c r="D72" s="0" t="s">
-        <v>1290</v>
+        <v>1665</v>
       </c>
       <c r="E72" s="0" t="s">
-        <v>1383</v>
+        <v>1758</v>
       </c>
       <c r="F72" s="0" t="s">
-        <v>1476</v>
+        <v>1851</v>
       </c>
       <c r="G72" s="0">
         <v>3</v>
@@ -6448,19 +7573,19 @@
         <v>3</v>
       </c>
       <c r="B73" s="0" t="s">
-        <v>1197</v>
+        <v>1572</v>
       </c>
       <c r="C73" s="0">
         <v>100</v>
       </c>
       <c r="D73" s="0" t="s">
-        <v>1291</v>
+        <v>1666</v>
       </c>
       <c r="E73" s="0" t="s">
-        <v>1384</v>
+        <v>1759</v>
       </c>
       <c r="F73" s="0" t="s">
-        <v>1477</v>
+        <v>1852</v>
       </c>
       <c r="G73" s="0">
         <v>0</v>
@@ -6474,19 +7599,19 @@
         <v>3</v>
       </c>
       <c r="B74" s="0" t="s">
-        <v>1198</v>
+        <v>1573</v>
       </c>
       <c r="C74" s="0">
         <v>100</v>
       </c>
       <c r="D74" s="0" t="s">
-        <v>1292</v>
+        <v>1667</v>
       </c>
       <c r="E74" s="0" t="s">
-        <v>1385</v>
+        <v>1760</v>
       </c>
       <c r="F74" s="0" t="s">
-        <v>1478</v>
+        <v>1853</v>
       </c>
       <c r="G74" s="0">
         <v>3</v>
@@ -6500,19 +7625,19 @@
         <v>3</v>
       </c>
       <c r="B75" s="0" t="s">
-        <v>1199</v>
+        <v>1574</v>
       </c>
       <c r="C75" s="0">
         <v>20</v>
       </c>
       <c r="D75" s="0" t="s">
-        <v>1293</v>
+        <v>1668</v>
       </c>
       <c r="E75" s="0" t="s">
-        <v>1386</v>
+        <v>1761</v>
       </c>
       <c r="F75" s="0" t="s">
-        <v>1479</v>
+        <v>1854</v>
       </c>
       <c r="G75" s="0">
         <v>2</v>
@@ -6526,19 +7651,19 @@
         <v>3</v>
       </c>
       <c r="B76" s="0" t="s">
-        <v>1200</v>
+        <v>1575</v>
       </c>
       <c r="C76" s="0">
         <v>40</v>
       </c>
       <c r="D76" s="0" t="s">
-        <v>1294</v>
+        <v>1669</v>
       </c>
       <c r="E76" s="0" t="s">
-        <v>1387</v>
+        <v>1762</v>
       </c>
       <c r="F76" s="0" t="s">
-        <v>1480</v>
+        <v>1855</v>
       </c>
       <c r="G76" s="0">
         <v>2</v>
@@ -6552,19 +7677,19 @@
         <v>1</v>
       </c>
       <c r="B77" s="0" t="s">
-        <v>1201</v>
+        <v>1576</v>
       </c>
       <c r="C77" s="0">
         <v>20</v>
       </c>
       <c r="D77" s="0" t="s">
-        <v>1295</v>
+        <v>1670</v>
       </c>
       <c r="E77" s="0" t="s">
-        <v>1388</v>
+        <v>1763</v>
       </c>
       <c r="F77" s="0" t="s">
-        <v>1481</v>
+        <v>1856</v>
       </c>
       <c r="G77" s="0">
         <v>0</v>
@@ -6578,19 +7703,19 @@
         <v>1</v>
       </c>
       <c r="B78" s="0" t="s">
-        <v>1202</v>
+        <v>1577</v>
       </c>
       <c r="C78" s="0">
         <v>120</v>
       </c>
       <c r="D78" s="0" t="s">
-        <v>1296</v>
+        <v>1671</v>
       </c>
       <c r="E78" s="0" t="s">
-        <v>1389</v>
+        <v>1764</v>
       </c>
       <c r="F78" s="0" t="s">
-        <v>1482</v>
+        <v>1857</v>
       </c>
       <c r="G78" s="0">
         <v>1</v>
@@ -6604,19 +7729,19 @@
         <v>1</v>
       </c>
       <c r="B79" s="0" t="s">
-        <v>1203</v>
+        <v>1578</v>
       </c>
       <c r="C79" s="0">
         <v>100</v>
       </c>
       <c r="D79" s="0" t="s">
-        <v>1297</v>
+        <v>1672</v>
       </c>
       <c r="E79" s="0" t="s">
-        <v>1390</v>
+        <v>1765</v>
       </c>
       <c r="F79" s="0" t="s">
-        <v>1483</v>
+        <v>1858</v>
       </c>
       <c r="G79" s="0">
         <v>1</v>
@@ -6630,19 +7755,19 @@
         <v>1</v>
       </c>
       <c r="B80" s="0" t="s">
-        <v>1204</v>
+        <v>1579</v>
       </c>
       <c r="C80" s="0">
         <v>60</v>
       </c>
       <c r="D80" s="0" t="s">
-        <v>1298</v>
+        <v>1673</v>
       </c>
       <c r="E80" s="0" t="s">
-        <v>1391</v>
+        <v>1766</v>
       </c>
       <c r="F80" s="0" t="s">
-        <v>1484</v>
+        <v>1859</v>
       </c>
       <c r="G80" s="0">
         <v>1</v>
@@ -6656,19 +7781,19 @@
         <v>1</v>
       </c>
       <c r="B81" s="0" t="s">
-        <v>1205</v>
+        <v>1580</v>
       </c>
       <c r="C81" s="0">
         <v>40</v>
       </c>
       <c r="D81" s="0" t="s">
-        <v>1299</v>
+        <v>1674</v>
       </c>
       <c r="E81" s="0" t="s">
-        <v>1392</v>
+        <v>1767</v>
       </c>
       <c r="F81" s="0" t="s">
-        <v>1485</v>
+        <v>1860</v>
       </c>
       <c r="G81" s="0">
         <v>1</v>
@@ -6682,19 +7807,19 @@
         <v>1</v>
       </c>
       <c r="B82" s="0" t="s">
-        <v>1206</v>
+        <v>1581</v>
       </c>
       <c r="C82" s="0">
         <v>80</v>
       </c>
       <c r="D82" s="0" t="s">
-        <v>1300</v>
+        <v>1675</v>
       </c>
       <c r="E82" s="0" t="s">
-        <v>1393</v>
+        <v>1768</v>
       </c>
       <c r="F82" s="0" t="s">
-        <v>1486</v>
+        <v>1861</v>
       </c>
       <c r="G82" s="0">
         <v>1</v>
@@ -6708,19 +7833,19 @@
         <v>1</v>
       </c>
       <c r="B83" s="0" t="s">
-        <v>1207</v>
+        <v>1582</v>
       </c>
       <c r="C83" s="0">
         <v>60</v>
       </c>
       <c r="D83" s="0" t="s">
-        <v>1301</v>
+        <v>1676</v>
       </c>
       <c r="E83" s="0" t="s">
-        <v>1394</v>
+        <v>1769</v>
       </c>
       <c r="F83" s="0" t="s">
-        <v>1487</v>
+        <v>1862</v>
       </c>
       <c r="G83" s="0">
         <v>2</v>
@@ -6734,19 +7859,19 @@
         <v>2</v>
       </c>
       <c r="B84" s="0" t="s">
-        <v>1208</v>
+        <v>1583</v>
       </c>
       <c r="C84" s="0">
         <v>100</v>
       </c>
       <c r="D84" s="0" t="s">
-        <v>1302</v>
+        <v>1677</v>
       </c>
       <c r="E84" s="0" t="s">
-        <v>1395</v>
+        <v>1770</v>
       </c>
       <c r="F84" s="0" t="s">
-        <v>1488</v>
+        <v>1863</v>
       </c>
       <c r="G84" s="0">
         <v>0</v>
@@ -6760,19 +7885,19 @@
         <v>2</v>
       </c>
       <c r="B85" s="0" t="s">
-        <v>1209</v>
+        <v>1584</v>
       </c>
       <c r="C85" s="0">
         <v>60</v>
       </c>
       <c r="D85" s="0" t="s">
-        <v>1303</v>
+        <v>1678</v>
       </c>
       <c r="E85" s="0" t="s">
-        <v>1396</v>
+        <v>1771</v>
       </c>
       <c r="F85" s="0" t="s">
-        <v>1489</v>
+        <v>1864</v>
       </c>
       <c r="G85" s="0">
         <v>1</v>
@@ -6786,19 +7911,19 @@
         <v>2</v>
       </c>
       <c r="B86" s="0" t="s">
-        <v>1210</v>
+        <v>1585</v>
       </c>
       <c r="C86" s="0">
         <v>100</v>
       </c>
       <c r="D86" s="0" t="s">
-        <v>1304</v>
+        <v>1679</v>
       </c>
       <c r="E86" s="0" t="s">
-        <v>1397</v>
+        <v>1772</v>
       </c>
       <c r="F86" s="0" t="s">
-        <v>1490</v>
+        <v>1865</v>
       </c>
       <c r="G86" s="0">
         <v>2</v>
@@ -6812,19 +7937,19 @@
         <v>2</v>
       </c>
       <c r="B87" s="0" t="s">
-        <v>1211</v>
+        <v>1586</v>
       </c>
       <c r="C87" s="0">
         <v>120</v>
       </c>
       <c r="D87" s="0" t="s">
-        <v>1305</v>
+        <v>1680</v>
       </c>
       <c r="E87" s="0" t="s">
-        <v>1398</v>
+        <v>1773</v>
       </c>
       <c r="F87" s="0" t="s">
-        <v>1491</v>
+        <v>1866</v>
       </c>
       <c r="G87" s="0">
         <v>2</v>
@@ -6838,19 +7963,19 @@
         <v>2</v>
       </c>
       <c r="B88" s="0" t="s">
-        <v>1212</v>
+        <v>1587</v>
       </c>
       <c r="C88" s="0">
         <v>60</v>
       </c>
       <c r="D88" s="0" t="s">
-        <v>1306</v>
+        <v>1681</v>
       </c>
       <c r="E88" s="0" t="s">
-        <v>1399</v>
+        <v>1774</v>
       </c>
       <c r="F88" s="0" t="s">
-        <v>1492</v>
+        <v>1867</v>
       </c>
       <c r="G88" s="0">
         <v>4</v>
@@ -6864,19 +7989,19 @@
         <v>3</v>
       </c>
       <c r="B89" s="0" t="s">
-        <v>1213</v>
+        <v>1588</v>
       </c>
       <c r="C89" s="0">
         <v>100</v>
       </c>
       <c r="D89" s="0" t="s">
-        <v>1307</v>
+        <v>1682</v>
       </c>
       <c r="E89" s="0" t="s">
-        <v>1400</v>
+        <v>1775</v>
       </c>
       <c r="F89" s="0" t="s">
-        <v>1493</v>
+        <v>1868</v>
       </c>
       <c r="G89" s="0">
         <v>3</v>
@@ -6890,19 +8015,19 @@
         <v>3</v>
       </c>
       <c r="B90" s="0" t="s">
-        <v>1214</v>
+        <v>1589</v>
       </c>
       <c r="C90" s="0">
         <v>60</v>
       </c>
       <c r="D90" s="0" t="s">
-        <v>1308</v>
+        <v>1683</v>
       </c>
       <c r="E90" s="0" t="s">
-        <v>1401</v>
+        <v>1776</v>
       </c>
       <c r="F90" s="0" t="s">
-        <v>1494</v>
+        <v>1869</v>
       </c>
       <c r="G90" s="0">
         <v>4</v>
@@ -6916,19 +8041,19 @@
         <v>3</v>
       </c>
       <c r="B91" s="0" t="s">
-        <v>1215</v>
+        <v>1590</v>
       </c>
       <c r="C91" s="0">
         <v>60</v>
       </c>
       <c r="D91" s="0" t="s">
-        <v>1309</v>
+        <v>1684</v>
       </c>
       <c r="E91" s="0" t="s">
-        <v>1402</v>
+        <v>1777</v>
       </c>
       <c r="F91" s="0" t="s">
-        <v>1495</v>
+        <v>1870</v>
       </c>
       <c r="G91" s="0">
         <v>3</v>
@@ -6942,19 +8067,19 @@
         <v>3</v>
       </c>
       <c r="B92" s="0" t="s">
-        <v>1216</v>
+        <v>1591</v>
       </c>
       <c r="C92" s="0">
         <v>120</v>
       </c>
       <c r="D92" s="0" t="s">
-        <v>1310</v>
+        <v>1685</v>
       </c>
       <c r="E92" s="0" t="s">
-        <v>1403</v>
+        <v>1778</v>
       </c>
       <c r="F92" s="0" t="s">
-        <v>1496</v>
+        <v>1871</v>
       </c>
       <c r="G92" s="0">
         <v>3</v>
@@ -6968,19 +8093,19 @@
         <v>3</v>
       </c>
       <c r="B93" s="0" t="s">
-        <v>1217</v>
+        <v>1592</v>
       </c>
       <c r="C93" s="0">
         <v>120</v>
       </c>
       <c r="D93" s="0" t="s">
-        <v>1311</v>
+        <v>1686</v>
       </c>
       <c r="E93" s="0" t="s">
-        <v>1404</v>
+        <v>1779</v>
       </c>
       <c r="F93" s="0" t="s">
-        <v>1497</v>
+        <v>1872</v>
       </c>
       <c r="G93" s="0">
         <v>1</v>

</xml_diff>